<commit_message>
fixed remove row, added undo + redo
</commit_message>
<xml_diff>
--- a/template_sekundarstufe_1-backup.xlsx
+++ b/template_sekundarstufe_1-backup.xlsx
@@ -455,7 +455,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>47 (151.6%)</t>
+          <t>27 (87.1%)</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -471,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -514,19 +514,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>9 (29.0%)</t>
+          <t>14 (45.2%)</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>

</xml_diff>